<commit_message>
updated by 20140227 created document and view architecture2 updated the HTTP/1.1 matrix
</commit_message>
<xml_diff>
--- a/HTTP1.1消息头定义及其与方法的对应关系.xlsx
+++ b/HTTP1.1消息头定义及其与方法的对应关系.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="135" windowWidth="19395" windowHeight="7605" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="19395" windowHeight="7575" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.1.Collected Grammar" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <t>Accept</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -232,10 +232,6 @@
   </si>
   <si>
     <t>WWW-Authenticate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用于：服务驱动的交涉（Server-driven Negotiation）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -462,7 +458,6 @@
   </si>
   <si>
     <t>字符集
-HTTP uses the same definition of the term “character set” as that described for MIME:
 HTTP使用在MIME中定义的名词“字符集（character set）”的含义。
 The term “character set” is used in this document to refer to a method used with one or more tables to
 convert a sequence of octets into a sequence of characters. Note that unconditional conversion in the other
@@ -493,12 +488,546 @@
 recipient’s preference, when initially displaying a document. See section 3.7.1.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Extension Header Fields</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accept-Language = "Accept-Language" ":"
+                   1#( language-range [ ";" "q" "=" qvalue ] )
+language-range  = ( ( 1*8ALPHA *( "-" 1*8ALPHA ) ) | "*" )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accept-Encoding: compress, gzip
+Accept-Encoding:
+Accept-Encoding: *
+Accept-Encoding: compress;q=0.5, gzip;q=1.0
+Accept-Encoding: gzip;q=1.0, identity; q=0.5, *;q=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   内容代码（content-coding）：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>内容代码指示一种已经或者能够被应用到实体（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>entity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）上编码转换。内容代码主要用于文档被在不丢失标识且不丢失信息的前提下被压缩或者被进行有用的转换。通常，实体被以编码的形式存储（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>document is stored in coded form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>），然后被直接传输，只有接受者才解码</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(decode)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    内容代码的NBF格式：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>content-coding = token
+    内容代码值是大小写不敏感的。HTTP 1.1在Accept-Encoding与Content-Encoding这两个头域中使用内容代码。尽管值是用来描述内容代码的，但它最终要的作用是用来指示解除编码需要使用哪种解码机制。
+    IANA负责内容编码的注册管理工作。初始的内容编码包括以下几项：
+    gzip：由文件压缩程序gzip(GNU gzip)提供的编码格式。参考RFC 1952获取详细信息。这种格式是带有32位循环冗余校验码（CRC）的Lempel-Ziv代码。
+    compress：由通用UNIX文件压缩程序compress提供的编码格式。这是一种Lempel-Ziv-Welch编码(LZW).
+      我们并不希望也不鼓励在今后的编码中使用应用程序名作为编码格式的指示符。应当考虑使用替代的x-gzip和x-compress
+    deflate：RFC 1950 [31]中所定义的zlib与RFC 1951 [29]中所定义的deflate压缩机制的联合体。
+    identity：默认的代码。表示不进行任何转换。这个内容代码只能用于Accept-Encoding头，不应当被用于Content-Encoding头。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Accept-Encoding = "Accept-Encoding" ":"
+                   1#( codings [ ";" "q" "=" qvalue ] )
+codings         = ( content-coding | "*" )
+content-coding  = token    ;参考</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>内容代码</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    [概要说明]Accept-Encoding请求头域，与Accept相似。但是约束了响应（Response）中的可接受的内容编码（content-coding）。
+用于：服务驱动的交涉（Server-driven Negotiation）
+    服务器使用如下规则，根据Accept-Encoding头域，测试是否一个内容代码可被接受：
+    1.如果这个内容编码是Accept-Encoding中所列出的其中一种，那么它是可接受的，除非它附加着一个值为0的qvalue。
+    2.星号“*”表示匹配在Accept-Encoding头域中没有明确列举的其它任何有效的内容代码。
+    3.如果有多个内容代码是可接受的，那么优先选取qvalue值最大的那个。
+    4.内容编码“identity”总是被接受的，除了以下两种情况：1)在Accept-Encoding中通过“identity;q=0”来明确表示不接受它；2)该域包含“*;q=0”并且没有明确表示接受identity。如果Accept-Encoding头域值为空，那么只有identity这个内容代码是可接受的。
+    如果Accept-Encoding头域出现在请求中，并且服务端无法返回一个匹配它的响应，那么服务端应该返回一个包含406错误代码的响应。
+    如果</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>没有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Accept-Encoding头域出现在请求中，服务端会假设所有内容代码都是可为客户端所接受的。这种情况下，identity是其中一种内容代码，服务器应该使用它，除非服务器端有额外的信息表明对于客户端来说别的内容编码是有意义的。
+注意：
+1.如果请求中没有包含Accept-Encoding，并且如果内容代码identity是无效的，则通常使用HTTP 1.0的客户端能够识别的内容编码（比如gzip和compress）；一些老的客户端会用其它内容代码显示出不正确的信息。服务器端应当基于特定的用户代理或客户端来做出决定。
+2.协议HTTP 1.0不认识或者说不遵从qvalue约定。这也就是说对于x-gzip和x-compress来说qvalue不起作用。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Accept-Language: da, en-gb;q=0.8, en;q=0.7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+我想要丹麦语（Danish），但也可以接受英格兰英语（British English）或者其它类型的英语。
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Language-Tag</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>language tag定义了由人类表达的用于与其它人交流沟通的自然语言的口语、书面语或者其它方面。不包括计算机语言。
+HTTP 1.1在Accept-Language和Content-Language域中使用language tag。
+    HTTP语言的语法与注册，同RFC 1766 [1].中的定义一样。简单来说，language tag由一个或多个部分组成：主language tag和可能为空的子tag系列。
+    language-tag = primary-tag *( "-" subtag )
+    primary-tag  = 1*8ALPHA
+    subtag       = 1*8ALPHA
+    tag中不允许空白，并且是大小写不敏感的。
+    language tags的命名是由IANA管理的。比如：en, en-US, en-cockney, i-cherokee, x-pig-latin，其中任何两位的主tag是ISO-639语言的缩写，任何两位的副tag是ISO-3166国家代码。（最后三个不是已注册的，但他们是一个非常好的例子，代表以后可能会被注册的样子）。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    [概要说明]Accept-Language头域类似于Accept，但是限定了客户端希望被用到响应中的自然语言集。
+    每一个language-range应当被关联一个quality value，来表示对用户偏爱由那个range所定义的语言的程度的评估。Quality value的默认值是1。
+    一个language-range匹配一个language-tag如果它等于这个tag的话，或者如果它等于这个tag的前缀（第一个后面为字符“-”的tag字符）。特殊的range“*”，如果它出现在Accept-Language里的话，代表匹配所有Accept-Language中所定义的tag以外的所有tag。
+    用于：服务驱动的交涉（Server-driven Negotiation）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    排列单位（Range Unit）
+    HTTP/1.1允许客户端请求响应实体的一部分。HTTP/1.1在Range和Content-Range头域中使用range units。根据多种结构化的单位（unit），一个响应实体可以被分解为多个部分。
+    range-unit       = bytes-unit | other-range-unit
+    bytes-unit       = "bytes"
+    other-range-unit = token
+    HTTP/1.1只定义了“bytes”这一个单位。HTTP1/1.1的实现者可以忽略由其它单位（units）定义的排列（ranges）。
+    HTTP/1.1已经被定义为允许实现不依赖Range相关知识的应用。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accept-Ranges     = "Accept-Ranges" ":" acceptable-ranges
+acceptable-ranges = 1#range-unit | "none"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accept-Ranges: bytes
+Accept-Ranges: none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>request-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>response-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>request-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    [概要说明]响应头域中的Accept-Ranges允许服务端指示它能接受的对于一个资源的Range请求（Range Request）。
+    接受byte-range请求的源服务端可以发送：
+    Accept-Ranges: bytes
+    但你也没必要发送该请求，以为客户端即使没有收到某资源的报头信息也可以实现byte-range请求。
+    而发送：
+    Accept-Ranges: none
+    ，则提示客户端：不建议使用Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age        = "Age" ":" age-value
+age-value  = delta-seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13.2.3 Age Calculations
+In order to know if a cached entry is fresh, a cache needs to know if its age exceeds its freshness lifetime. We discuss
+how to calculate the latter in section 13.2.4; this section describes how to calculate the age of a response or cache
+entry.
+In this discussion, we use the term “now” to mean “the current value of the clock at the host performing the
+calculation.” Hosts that use HTTP, but especially hosts running origin servers and caches, SHOULD use NTP [28]
+or some similar protocol to synchronize their clocks to a globally accurate time standard.
+HTTP/1.1 requires origin servers to send a Date header, if possible, with every response, giving the time at which
+the response was generated (see section 14.18). We use the term “date_value” to denote the value of the Date
+header, in a form appropriate for arithmetic operations.
+HTTP/1.1 uses the Age response-header to convey the estimated age of the response message when obtained from a
+cache. The Age field value is the cache’s estimate of the amount of time since the response was generated or
+revalidated by the origin server.
+In essence, the Age value is the sum of the time that the response has been resident in each of the caches along the
+path from the origin server, plus the amount of time it has been in transit along network paths.
+We use the term “age_value” to denote the value of the Age header, in a form appropriate for arithmetic operations.
+A response’s age can be calculated in two entirely independent ways:
+1. now minus date_value, if the local clock is reasonably well synchronized to the origin server’s clock. If the
+result is negative, the result is replaced by zero.
+2. age_value, if all of the caches along the response path implement HTTP/1.1.
+Given that we have two independent ways to compute the age of a response when it is received, we can combine
+these as
+corrected_received_age = max(now - date_value, age_value)
+and as long as we have either nearly synchronized clocks or all-HTTP/1.1 paths, one gets a reliable (conservative)
+result.
+RFC 2616 HTTP/1.1 June, 1999
+Fielding, et al Standards Track [Page 52]
+Because of network-imposed delays, some significant interval might pass between the time that a server generates a
+response and the time it is received at the next outbound cache or client. If uncorrected, this delay could result in
+improperly low ages.
+Because the request that resulted in the returned Age value must have been initiated prior to that Age value’s
+generation, we can correct for delays imposed by the network by recording the time at which the request was
+initiated. Then, when an Age value is received, it MUST be interpreted relative to the time the request was initiated,
+not the time that the response was received. This algorithm results in conservative behavior no matter how much
+delay is experienced. So, we compute:
+corrected_initial_age = corrected_received_age
++ (now - request_time)
+where “request_time” is the time (according to the local clock) when the request that elicited this response was sent.
+Summary of age calculation algorithm, when a cache receives a response:
+/*
+* age_value
+* is the value of Age: header received by the cache with
+* this response.
+* date_value
+* is the value of the origin server's Date: header
+* request_time
+* is the (local) time when the cache made the request
+* that resulted in this cached response
+* response_time
+* is the (local) time when the cache received the
+* response
+* now
+* is the current (local) time
+*/
+apparent_age = max(0, response_time - date_value);
+corrected_received_age = max(apparent_age, age_value);
+response_delay = response_time - request_time;
+corrected_initial_age = corrected_received_age + response_delay;
+resident_time = now - response_time;
+current_age = corrected_initial_age + resident_time;
+The current_age of a cache entry is calculated by adding the amount of time (in seconds) since the cache entry
+was last validated by the origin server to the corrected_initial_age. When a response is generated from a
+cache entry, the cache MUST include a single Age header field in the response with a value equal to the cache
+entry's current_age.
+The presence of an Age header field in a response implies that a response is not first-hand. However, the converse is
+not true, since the lack of an Age header field in a response does not imply that the response is first-hand unless all
+caches along the request path are compliant with HTTP/1.1 (i.e., older HTTP caches did not implement the Age
+header field).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    [概要说明]响应头域中的Age表达了发送者对从渊服务端生成响应开始的总时间的评估。
+    一个缓存的“响应”是“新鲜的”，如果它的Age不超过它的新鲜生命周期。（Age的计算请参照“参考”栏）
+    Age是非负整数，代表秒。
+    如果缓存收到大于正整数最大值的数值，或者在Age计算过程中溢出了的话，那么它</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>必须</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>传输2147483648 (2^31)。
+    一个包含了缓存的HTTP/1.1服务器必须在由其自身缓存生成的响应中包含一个Age头域。
+    缓存应当使用一个至少31位的算数类型。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Allow = "Allow" ":" #Method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Allow: GET, HEAD, PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>entity-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    [概要说明]实体头域Allow列出了由Request-URI定义的资源所支持的方法。这个头域的目的是严格地通知接受者资源所关联的有效方法。
+    当响应状态是405 (Method Not Allowed)时，Allow头域必须出现在响应头域中。
+    这个头域无法阻止客户端尝试其它方法，但是在Allow头域中出现的指示应当被遵从。实际的所允许的方法集由源服务器在每次请求来到时定义。
+    代理必须不要修改Allow头域，即使它不理解所有定义的方法，因为用户代理可能有其它的与源服务器交流的意思。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Authorization = "Authorization" ":" credentials</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    [概要说明]用户代理通常（但不是必须）在收到一个401（Unauthorized）错误后，可能希望证明他们自己——通过使用Authorization请求头域。
+    Authorization域的值由credentials构成。Credentials包含针对被请求的资源相关的客户代理的认证信息。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,6 +1060,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -546,7 +1084,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -673,13 +1211,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -687,15 +1264,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -738,6 +1306,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3834,7 +4417,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3892,17 +4475,17 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -3913,476 +4496,607 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="66.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="56.125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="2"/>
+    <col min="2" max="2" width="23.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="55.375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="66.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="56.125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="351" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="351" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="3" spans="1:6" ht="292.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17" t="s">
+      <c r="E3" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="18" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="243" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="189" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="203.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="10"/>
+    </row>
+    <row r="50" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="10"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="13"/>
+    <row r="51" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="17"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52" s="5"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
updated http header definition
updated http header definition (general-header)
</commit_message>
<xml_diff>
--- a/HTTP1.1消息头定义及其与方法的对应关系.xlsx
+++ b/HTTP1.1消息头定义及其与方法的对应关系.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="19395" windowHeight="7575" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="195" windowWidth="19395" windowHeight="7545" tabRatio="735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.1.Collected Grammar" sheetId="4" r:id="rId1"/>
     <sheet name="1.2.Method Definitions" sheetId="2" r:id="rId2"/>
     <sheet name="1.3.Header Field List" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="1.3.1.Cache-Control头域详解" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'1.3.Header Field List'!$A$1:$F$47</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="122">
   <si>
     <t>Accept</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,18 +78,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Allow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Authorization</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cache-Control</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Connection</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -220,14 +211,6 @@
   </si>
   <si>
     <t>Vary</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Via</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Warining</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -859,10 +842,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>request-header</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>response-header</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1022,12 +1001,279 @@
     Authorization域的值由credentials构成。Credentials包含针对被请求的资源相关的客户代理的认证信息。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Authorization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Allow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">general-header </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>request-header</t>
+  </si>
+  <si>
+    <t>request-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>response-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>entity-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Via</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Warining</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>request-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">general-header </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>entity-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>response-header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cache-Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cache-Control           = "Cache-Control" ":" 1#cache-directive
+cache-directive         = cache-request-directive
+                          | cache-response-directive
+cache-request-directive =
+                  "no-cache"                             ; Section 14.9.1
+                | "no-store"                             ; Section 14.9.2
+                | "max-age" "=" delta-seconds    ; Section 14.9.3, 14.9.4
+                | "max-stale" [ "=" delta-seconds ]      ; Section 14.9.3
+                | "min-fresh" "=" delta-seconds          ; Section 14.9.3
+                | "no-transform"                         ; Section 14.9.5
+                | "only-if-cached"                       ; Section 14.9.4
+                | cache-extension                        ; Section 14.9.6
+cache-response-directive =
+                "public"                                 ; Section 14.9.1
+                | "private" [ "=" &lt;"&gt; 1#field-name &lt;"&gt; ] ; Section 14.9.1
+                | "no-cache" [ "=" &lt;"&gt; 1#field-name &lt;"&gt; ]; Section 14.9.1
+                | "no-store"                             ; Section 14.9.2
+                | "no-transform"                         ; Section 14.9.5
+                | "must-revalidate"                      ; Section 14.9.4
+                | "proxy-revalidate"                     ; Section 14.9.4
+                | "max-age" "=" delta-seconds            ; Section 14.9.3
+                | "s-maxage" "=" delta-seconds           ; Section 14.9.3
+                | cache-extension                        ; Section 14.9.6
+cache-extension         = token [ "=" ( token | quoted-string ) ]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cache-control指令可以被分解以下几类：
+1.限制哪些东西是可缓存的；这个可能只由源服务器提出；
+2.限制哪些东西应当被保存到缓存。这个可以由源服务器或用户提出。
+3.对基本的过期机制的修改。这个可以由源服务器或用户提出。
+4.对再次验证缓存与再次加载缓存的控制。这个一般由用户提出。
+5.对实体传输的控制。
+6.对缓存系统的扩展。
+下面对每一类加以说明：
+1.What is Cacheable
+2.What May be Stored by Caches
+3.Modifications of the Basic Expiration Mechanism
+4.Cache Revalidation and Reload Controls
+5.No-Transform Directive
+6.Cache Control Extensions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    [概要说明]Cache-Control这一general-header头域是用来定义一些必须请求/响应链条上的服务器所必需响应的指示的。这些指令定义一些行为以防止缓存对请求/响应产生一些不利的干预干涉。
+    注意：HTTP/1.0缓存可能不会实现Cache-Control，而只有Pragma:no-cache这一实现。
+    缓存指示必需能够在被传递时穿透代理或者网关应用程序，不管它们对于这些应用程序的重要性如何，因为这些指示必需能够被应用到请求响应链上的所有接收者。为一个特别的缓存定义缓存指令是不可能的。
+    当一个指令里面没有任何一个1#field-name的时候，这个指令应用于整个请求或响应。当指令里含有1#field-name时，这个指令只应用到命名的域，而不是这个请求或响应的其它域。这个机制是可扩展的；HTTP协议的未来版本的实现可能应用这些指令到HTTP/1.1中没有定义的头域中。
+    cache-control指令可以被分解以下几类：
+    1.限制哪些东西是可缓存的；这个可能只由源服务器提出；
+    2.限制哪些东西应当被保存到缓存。这个可以由源服务器或用户提出。
+    3.对基本的过期机制的修改。这个可以由源服务器或用户提出。
+    4.对再次验证缓存与再次加载缓存的控制。这个一般由用户提出。
+    5.对实体传输的控制。
+    6.对缓存系统的扩展。
+各个分类的详细说明，请参考“1.3.1.Cache-Control头域详解”一页。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connection = "Connection" ":" 1#(connection-token)
+connection-token = token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connection: close</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    [概要说明]通用头域Connection允许发送者定义一些期望特定的连接能拥有的选项，并且必须不会被代理扩散到以后的连接上去。
+    HTTP/1.1代理在转送此消息之前，必须解析该头域，并且移除该消息头域中与该头域中的connection-token重名的头域（可能有多个）。
+    Connection的连接选项由connection-token定义，而不是由其它对应的额外头域定义，因为其它对应的额外头域可能不会被传送，如果它们没有与选项相关联的参数的话。
+    被罗列在Connection头中的消息报头中，必须不包含end-to-end报头，诸如Cache-Control。
+    HTTP/1.1定义了一个close连接选项，发送者可以用它来发出要求连接在响应完成后将被关闭这样的信号。比如在请求或者响应头包含“Connection: close”，来指示这个连接在请求响应结束后，不应当被认为是持久的了。
+    HTTP/1.1应用程序如果不支持持久化连接的话，必须在任何的消息头中包含close连接选项。
+    系统收到HTTP/1.0或者更低版本的包含Connection头域的消息的话，必须移除或者忽略该消息中的任何一个与连接选项名相同的头域，以保护这些头域被早期HTTP协议代理误转发了（兼容早期协议）。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date = "Date" ":" HTTP-date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date: Tue, 15 Nov 1994 08:12:31 GMT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    [概要说明]通用头域Date代表消息是在哪个时间点被创建的，其语法与RFC 822中定义的语法一样。该域的值是一个HTTP-date，它必须是RFC 1123 [8]日期格式。
+    源服务器必须为每一个响应添加Date头域，除了以下情况：
+    1.如果响应状态码是100 (Continue)或者101 (Switching Protocols)的话，根据服务端的选项，响应可能包含一个Date头域。
+    2.如果响应状态码显示一个服务端错误，比如500 (Internal Server Error)或者503 (Service Unavailable)，并且很难或者不可能生成一个Date时。
+    3.如果服务端没有能够提供当前时间近似值的时钟时，响应消息头域必须不含Date。此时应该遵守其它规范（※１）
+    如果收到的消息中不含Date,那么如果该消息将要被缓存，或者会被以某个需要Date的协议网管传递的话，则接收者必须为这个消息添加Date。
+    一个没有时钟的HTTP实现，在缓存消息前，必须每次都重新验证消息。一个缓存，尤其是共享缓存，必须采用一些机制，比如NTP，来同步时间为国际标准。
+    客户端应当仅在消息中含有实体时才添加Date，比如在发出PUT和POST请求时。客户端没有时钟的话必须不添加Date.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>※１没有时钟的源服务器不应当为Expires 或 Last-Modified赋值。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pragma = "Pragma" ":" 1#pragma-directive
+pragma-directive = "no-cache" | extension-pragma
+extension-pragma = token [ "=" ( token | quoted-string ) ]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pragma: no-cache</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    [概要说明]通用头域Pragma是用来包含可能被应用到请求响应链上的任何一个接收者的具体实现方面的指示。所有的Pragma指示定义了从协议角度看待的可选行为；不过一些系统可能要求行为与指示一致。
+    当一个no-cache指示出现在请求消息中时，应用应该转发这个请求到源服务器，尽管该应用有拷贝所请求的对象至缓存的功能。这个paragma指示与catche指示中的no-cache有相同的语义，这个paragma指示被定义在这儿是为了兼容HTTP/1.0。当向不知道能够兼容HTTP/1.1的服务器发送no-cache请求时，客户端应当包含这2个报头。
+    Pragma指示必需能够在被传递时穿透代理或者网关应用程序，不管它们对于这些应用程序的重要性如何，因为这些指示必需能够被应用到请求响应链上的所有接收者。为一个特别的缓存定义缓存指令是不可能的。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trailer = "Trailer" ":" 1#field-name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transfer-Encoding = "Transfer-Encoding" ":" 1#transfer-coding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    [概要说明]通用头域Transfer-Encoding指示为了安全地在发送者和接受者之间传输，哪种传输类型（if any）已经被应用到了消息体（message body）中了。
+    这个不同于content-encoding。Transfer-Encoding是消息（message）的属性，而不是实体（entity）的。
+    如果多种编码被应用到实体上了，那么Transfer-Encoding必须被按照它们的应用优选度列举出来。关于编码参数的附加信息，可能包含在非HTTP/1.1协议文档内所定义的头域中。
+    许多旧的HTTP/1.0应用不能理解Transfer-Encoding。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    [概要说明]通用头域Trailer指示指定的头域集合出现在以chunked这一传输码编码的消息的尾部（Trailer）中。
+    HTTP/1.1消息中应当包含一个使用Trunked传输码且是非空值的Trailer报头。这么做让接受者知道哪些头域是希望出现在尾部（Trailer）中的。
+    如果没有Trailer出现在头域中，那么尾部（Trailer）不应当包含任何头域</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+   列举在Trailer头域中的头域必须不包含：
+    1.Transfer-Encoding
+    2.Content-Length
+    3.Trailer</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>chunked transfer-coding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+transfer-coding        = "chunked" | transfer-extension
+transfer-extension     = token *( ";" parameter )
+parameter              = attribute "=" value
+attribute              = token
+value                  = token | quoted-string</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transfer-Encoding: chunked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1069,8 +1315,33 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1080,6 +1351,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1256,7 +1539,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1323,11 +1606,80 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4409,15 +4761,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -4475,17 +4827,17 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -4496,11 +4848,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4518,19 +4873,19 @@
         <v>3</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="351" x14ac:dyDescent="0.15">
@@ -4538,19 +4893,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="292.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -4558,19 +4913,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.15">
@@ -4578,19 +4933,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="243" x14ac:dyDescent="0.15">
@@ -4598,19 +4953,19 @@
         <v>11</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>76</v>
-      </c>
       <c r="F5" s="15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="189" x14ac:dyDescent="0.15">
@@ -4618,19 +4973,19 @@
         <v>12</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="203.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -4638,78 +4993,94 @@
         <v>13</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>95</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="409.5" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+        <v>103</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="E10" s="12"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="283.5" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="12"/>
@@ -4717,9 +5088,11 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="12"/>
@@ -4727,9 +5100,11 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="12"/>
@@ -4737,9 +5112,11 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="12"/>
@@ -4747,9 +5124,11 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="12"/>
@@ -4757,29 +5136,41 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="12"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="324" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="12"/>
+        <v>21</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="12"/>
@@ -4787,9 +5178,11 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="12"/>
@@ -4797,9 +5190,11 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="12"/>
@@ -4807,9 +5202,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="12"/>
@@ -4817,9 +5214,11 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="12"/>
@@ -4827,9 +5226,11 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="12"/>
@@ -4837,9 +5238,11 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="12"/>
@@ -4847,9 +5250,11 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="12"/>
@@ -4857,9 +5262,11 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="12"/>
@@ -4867,9 +5274,11 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="12"/>
@@ -4877,9 +5286,11 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="12"/>
@@ -4887,9 +5298,11 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="12"/>
@@ -4897,29 +5310,41 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="12"/>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="189" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>114</v>
+      </c>
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="12"/>
@@ -4927,9 +5352,11 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="6"/>
+        <v>37</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="12"/>
@@ -4937,9 +5364,11 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="12"/>
@@ -4947,9 +5376,11 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="12"/>
@@ -4957,9 +5388,11 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="12"/>
@@ -4967,9 +5400,11 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="12"/>
@@ -4977,51 +5412,71 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="12"/>
       <c r="F39" s="7"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="152.25" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="E40" s="12"/>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F40" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>121</v>
+      </c>
       <c r="F41" s="7"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="7"/>
+      <c r="A42" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="25"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="12"/>
@@ -5029,41 +5484,45 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="C44" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="12"/>
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="7"/>
+      <c r="A45" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="25"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="7"/>
+      <c r="A46" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="25"/>
     </row>
     <row r="47" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="13"/>
@@ -5071,7 +5530,7 @@
     </row>
     <row r="50" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -5099,9 +5558,30 @@
       <c r="F53" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F47"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>"request-header"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"general-header "</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"entity-header"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"response-header"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"response-header"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5109,10 +5589,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="89.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="273" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>